<commit_message>
Reporte de vehiculos terminado
</commit_message>
<xml_diff>
--- a/templates/export/devices.xlsx
+++ b/templates/export/devices.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50FFA575-2173-4A27-B2CB-A590F248D44B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF92B1B-9B2C-421C-A51B-16FCB864ABF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="989" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
     <author>Autor</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -35,11 +35,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>jx:area(lastCell="F12")</t>
+          <t>jx:area(lastCell="J11")</t>
         </r>
       </text>
     </comment>
-    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -49,11 +49,11 @@
             <family val="2"/>
             <charset val="204"/>
           </rPr>
-          <t>jx:each(items="devices", var="device", lastCell="F12" multisheet="sheetNames")</t>
+          <t>jx:each(items="devices", var="device", lastCell="J11" multisheet="sheetNames")</t>
         </r>
       </text>
     </comment>
-    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{276DFE7F-860B-46CB-B369-55C93F051267}">
       <text>
         <r>
           <rPr>
@@ -63,7 +63,21 @@
             <family val="2"/>
             <charset val="204"/>
           </rPr>
-          <t>jx:each(items="device.objects", var="device", lastCell="F12")</t>
+          <t>jx:each(items="devices", var="device", lastCell="C11")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>jx:each(items="device.objects", var="device", lastCell="J11")</t>
         </r>
       </text>
     </comment>
@@ -72,37 +86,100 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Report type:</t>
-  </si>
-  <si>
-    <t>Devices</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>name</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="61"/>
+        <color rgb="FF324BAE"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>φ</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color rgb="FF324BAE"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>HI</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FF324BAE"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Project</t>
+    </r>
+  </si>
+  <si>
+    <t>${device.phone}</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Identificador</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>Modelo</t>
+  </si>
+  <si>
+    <t>Ultima Actualización</t>
+  </si>
+  <si>
+    <t>Telefono</t>
+  </si>
+  <si>
+    <t>Categoría</t>
   </si>
   <si>
     <t>${device.name}</t>
   </si>
   <si>
+    <t>${device.model}</t>
+  </si>
+  <si>
+    <t>${device.category}</t>
+  </si>
+  <si>
     <t>${device.status}</t>
   </si>
   <si>
-    <t>${device.id}</t>
+    <t>${device.uniqueId}</t>
+  </si>
+  <si>
+    <t>${dateTool.format("YYYY-MM-dd", device.lastUpdate, locale, timezone)}</t>
+  </si>
+  <si>
+    <t>${device.groupName}</t>
+  </si>
+  <si>
+    <t>Grupo</t>
+  </si>
+  <si>
+    <t>Vehículos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
+    <numFmt numFmtId="166" formatCode="0&quot; m&quot;"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -128,6 +205,13 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF444444"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -168,6 +252,45 @@
       <name val="Tahoma"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF324BAE"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF324BAE"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="61"/>
+      <color rgb="FF324BAE"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FF324BAE"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -196,7 +319,9 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top style="thin">
         <color auto="1"/>
       </top>
@@ -208,9 +333,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -218,24 +343,39 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="15"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -327,16 +467,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>285240</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>22380</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>207135</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>132870</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -384,16 +524,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>285240</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>22380</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>207135</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>132870</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -441,16 +581,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>285240</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>22380</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>207135</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>132870</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -498,15 +638,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>4019550</xdr:colOff>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -547,15 +687,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>4019550</xdr:colOff>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -596,15 +736,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>4019550</xdr:colOff>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -909,90 +1049,113 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="C1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625"/>
-    <col min="3" max="3" width="37" customWidth="1"/>
-    <col min="4" max="4" width="29.77734375" customWidth="1"/>
-    <col min="5" max="5" width="31" customWidth="1"/>
-    <col min="6" max="6" width="25.88671875" customWidth="1"/>
-    <col min="7" max="1020" width="8.6640625"/>
+    <col min="3" max="10" width="23.109375" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" customWidth="1"/>
+    <col min="12" max="12" width="19.88671875" customWidth="1"/>
+    <col min="13" max="13" width="20.33203125" customWidth="1"/>
+    <col min="14" max="1027" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B1" s="1"/>
-      <c r="C1" s="2"/>
+    <row r="1" spans="3:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="3:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="3:11" ht="76.2" x14ac:dyDescent="1.2">
+      <c r="F3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="G3" s="13"/>
+    </row>
+    <row r="4" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="F4" s="2"/>
+    </row>
+    <row r="6" spans="3:11" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="F6" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="14"/>
+    </row>
+    <row r="7" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="D7" s="1"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="9" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="D9" s="3"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="3:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="3:11" s="11" customFormat="1" ht="73.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="9" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B3" s="1"/>
-      <c r="C3" s="3"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B4" s="1"/>
-      <c r="C4" s="3"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="1"/>
-      <c r="C5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="1"/>
-      <c r="C6" s="3"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="1"/>
-      <c r="C7" s="3"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="1"/>
-      <c r="C8" s="3"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="1"/>
-      <c r="C9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="4"/>
-      <c r="C10" s="3"/>
-    </row>
-    <row r="11" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12"/>
-      <c r="B12" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E12"/>
-      <c r="F12"/>
+      <c r="I11" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F6:G6"/>
+  </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>